<commit_message>
2nd draft for cv, research statement
</commit_message>
<xml_diff>
--- a/List of position opennings.xlsx
+++ b/List of position opennings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="27940" windowHeight="17540"/>
+    <workbookView xWindow="880" yWindow="460" windowWidth="27920" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="106">
   <si>
     <t>Table 1</t>
   </si>
@@ -698,9 +698,6 @@
   <si>
     <t>Candidates with specific research expertise that contributes to the University’s emerging emphasis on intelligent infrastructure and smart design &amp; construction are particularly encouraged to apply. All faculty members in the CEE Department are expected to have a strong commitment to undergraduate teaching as well as to specialized graduate education. Likewise, they are expected to develop a strong record of scholarly work and sponsored research. The successful candidate will be appointed in the Vecellio Construction Engineering &amp; Management Program and will also have the opportunity to become a principal faculty member in the Myers-Lawson School of Construction. As such, the successful candidate will join a critical mass of faculty focused on research and education in construction and the built environment. Likewise, the CEE Department currently has 59 faculty members, with approximately 330 full-time graduate students and 550 undergraduate students. The Via Endowment allows the department to offer a significant number of scholarships and fellowships to highly qualified students.
 A successful candidate should be able to: (1) work across traditional boundaries in discovery, learning and engagement activities; (2) teach fundamental courses in infrastructure delivery, development and management; (3) sustain or develop a nationally recognized sponsored research program; (4) generate high impact scholarly work; and (5) contribute to the University’s emerging Intelligent Infrastructure for Human-Centered Communities Destination Area through research and teaching in thematic areas such as smart, sustainable cities and communities; smart construction; integrated energy systems; infrastructure network dynamics and engineering; cyber-physical systems; infrastructure resilience; or a related area.</t>
-  </si>
-  <si>
-    <t>North Carolina</t>
   </si>
   <si>
     <t>https://jobs.ncsu.edu/postings/75131</t>
@@ -811,6 +808,45 @@
   </si>
   <si>
     <t>Apply online at http://careers.rit.edu/faculty. Search: BR2737. Submit your cover letter addressing the listed qualifications; a vita; a contribution to diversityâ statement; and the names, addresses and phone numbers for three references.</t>
+  </si>
+  <si>
+    <t>Illinois State University</t>
+  </si>
+  <si>
+    <t>https://careers.insidehighered.com/job/1256974/assistant-professor-in-technology-management-/?TrackID=3&amp;utm_campaign=ZipAlerts&amp;utm_medium=cpc&amp;utm_source=ZipAlerts&amp;rx_campaign=zipalerts15&amp;rx_group=100135&amp;rx_job=1256974&amp;rx_medium=cpc&amp;rx_source=ZipAlerts#sc=jobfeed&amp;me=feed&amp;cm=Recruitics%20Feed</t>
+  </si>
+  <si>
+    <t>Iowa State University</t>
+  </si>
+  <si>
+    <t>https://www.iastatejobs.com/postings/22091#600192</t>
+  </si>
+  <si>
+    <t>california state university</t>
+  </si>
+  <si>
+    <t>open untill filled</t>
+  </si>
+  <si>
+    <t>http://www.startwire.com/express_apply_jobs/MjEyNF8xMjFiMzg1YzhmYWVjNTZiNzBlNTAxYzhlMTY2ZTIyZl9sdXVhX2k=?source=ziprecruiter_l2</t>
+  </si>
+  <si>
+    <t>The university of Delaware</t>
+  </si>
+  <si>
+    <t>Jannuary 27, 2017</t>
+  </si>
+  <si>
+    <t>https://apply.interfolio.com/38591</t>
+  </si>
+  <si>
+    <t>Applicants should submit (1) a cover letter summarizing the candidate’s interest in the position and relevant experience, (2) a complete resume or curriculum vitae, (3) a statement describing the candidate’s teaching philosophy with a list of courses that the candidate is qualified to teach, (4) a statement identifying areas of interest for research and/or professional involvement, and (5) the names and contact information of three references, at least one of whom can attest to the candidates teaching qualifications. Applicants should go to the website https://apply.interfolio.com/38591 to upload their information. In order to receive full consideration, applications should be received by January 27, 2017.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The successful applicant is expected to develop and deliver technical courses in the CE&amp;M curriculum, to mentor students and advise student organizations, to liaise with industry partners and program stakeholders and to maintain involvement in scholarly activities.The position is expected to be teaching and service oriented.  The successful candidate will have the opportunity to develop a limited research program in construction engineering, construction management or engineering education to complement and expand existing Departmental activities.</t>
+  </si>
+  <si>
+    <t>North Carolina State University</t>
   </si>
 </sst>
 </file>
@@ -2288,10 +2324,10 @@
   <dimension ref="A1:IV23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2508,7 +2544,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="224" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:12" ht="128" x14ac:dyDescent="0.15">
       <c r="A8" s="6"/>
       <c r="B8" s="14">
         <v>5</v>
@@ -2538,7 +2574,7 @@
       </c>
       <c r="L8" s="17"/>
     </row>
-    <row r="9" spans="1:12" ht="320" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:12" ht="224" x14ac:dyDescent="0.15">
       <c r="A9" s="6"/>
       <c r="B9" s="14">
         <v>6</v>
@@ -2632,35 +2668,35 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="192" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:12" ht="128" x14ac:dyDescent="0.15">
       <c r="A12" s="6"/>
       <c r="B12" s="14">
         <v>9</v>
       </c>
       <c r="C12" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="D12" s="17" t="s">
-        <v>72</v>
-      </c>
       <c r="E12" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F12" s="17"/>
       <c r="G12" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="H12" s="17" t="s">
-        <v>77</v>
-      </c>
       <c r="I12" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J12" s="17" t="s">
         <v>62</v>
       </c>
       <c r="K12" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L12" s="17"/>
     </row>
@@ -2670,60 +2706,60 @@
         <v>10</v>
       </c>
       <c r="C13" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="17" t="s">
         <v>78</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>79</v>
       </c>
       <c r="E13" s="21">
         <v>41211</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G13" s="17"/>
       <c r="H13" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I13" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J13" s="17"/>
       <c r="K13" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L13" s="17"/>
     </row>
-    <row r="14" spans="1:12" ht="384" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:12" ht="320" x14ac:dyDescent="0.15">
       <c r="A14" s="6"/>
       <c r="B14" s="14">
         <v>11</v>
       </c>
       <c r="C14" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="17" t="s">
         <v>84</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>85</v>
       </c>
       <c r="E14" s="22">
         <v>41257</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G14" s="17" t="s">
         <v>62</v>
       </c>
       <c r="H14" s="17"/>
       <c r="I14" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J14" s="17"/>
       <c r="K14" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L14" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="409" x14ac:dyDescent="0.15">
@@ -2732,50 +2768,64 @@
         <v>12</v>
       </c>
       <c r="C15" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="17" t="s">
         <v>90</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>91</v>
       </c>
       <c r="E15" s="22">
         <v>41196</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G15" s="17" t="s">
         <v>62</v>
       </c>
       <c r="H15" s="17"/>
       <c r="I15" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J15" s="17"/>
       <c r="K15" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L15" s="17"/>
     </row>
-    <row r="16" spans="1:12" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:12" ht="192" x14ac:dyDescent="0.15">
       <c r="A16" s="6"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
+      <c r="B16" s="14">
+        <v>13</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="21">
+        <v>41181</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>94</v>
+      </c>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
       <c r="I16" s="17"/>
       <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
       <c r="L16" s="17"/>
     </row>
-    <row r="17" spans="1:12" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:12" ht="32" x14ac:dyDescent="0.15">
       <c r="A17" s="6"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
+      <c r="B17" s="14">
+        <v>14</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D17" s="21">
+        <v>41227</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>96</v>
+      </c>
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
       <c r="H17" s="17"/>
@@ -2784,12 +2834,20 @@
       <c r="K17" s="17"/>
       <c r="L17" s="17"/>
     </row>
-    <row r="18" spans="1:12" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:12" ht="69" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="6"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
+      <c r="B18" s="14">
+        <v>15</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>99</v>
+      </c>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
       <c r="H18" s="17"/>
@@ -2798,18 +2856,30 @@
       <c r="K18" s="17"/>
       <c r="L18" s="17"/>
     </row>
-    <row r="19" spans="1:12" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:12" ht="208" x14ac:dyDescent="0.15">
       <c r="A19" s="6"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
+      <c r="B19" s="14">
+        <v>16</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>102</v>
+      </c>
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
+      <c r="H19" s="17" t="s">
+        <v>104</v>
+      </c>
       <c r="I19" s="17"/>
       <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
+      <c r="K19" s="17" t="s">
+        <v>103</v>
+      </c>
       <c r="L19" s="17"/>
     </row>
     <row r="20" spans="1:12" ht="22" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
2nd draft teaching statement
</commit_message>
<xml_diff>
--- a/List of position opennings.xlsx
+++ b/List of position opennings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="112">
   <si>
     <t>Table 1</t>
   </si>
@@ -847,6 +847,24 @@
   </si>
   <si>
     <t>North Carolina State University</t>
+  </si>
+  <si>
+    <t>East Carolina University</t>
+  </si>
+  <si>
+    <t>https://ecu.peopleadmin.com/applicants/jsp/shared/position/JobDetails_css.jsp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASSISTANT/ASSOCIATE PROFESSOR  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A minimum of three years of managerial experience in the construction industry; evidence of successful teaching in construction management at the college/university level; demonstrated ability to secure external funding, grants, and/or industry support and professional certification. Preference will be given to candidates able to teach courses in the following areas: Building Information Modeling (BIM), Mechanical, Electrical, and Plumbing (MEP) Systems, Estimating, Scheduling, and Cost Control, in face-to-face and distance learning environments. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">An earned PhD degree in Construction Management, Civil Engineering, or closely related field and a demonstrated potential to develop and sustain an active research agenda, effective communication and interpersonal skills; ability and desire to work in a team setting and make positive contributions to the department. All degrees must be from a regionally accredited institution. ABD may be considered for appointment at the rank of instructor and must provide documented evidence that their dissertation defense and completion of study is completed prior to the fall 2017 semester for fall 2017 hire. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Candidates must submit a cover letter, a curriculum vitae/resume, teaching statement, research statement and a list of three references, including contact information, online.  </t>
   </si>
 </sst>
 </file>
@@ -2324,10 +2342,10 @@
   <dimension ref="A1:IV23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="I19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2747,14 +2765,14 @@
       <c r="F14" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="G14" s="17" t="s">
-        <v>62</v>
-      </c>
+      <c r="G14" s="17"/>
       <c r="H14" s="17"/>
       <c r="I14" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="J14" s="17"/>
+      <c r="J14" s="17" t="s">
+        <v>62</v>
+      </c>
       <c r="K14" s="17" t="s">
         <v>86</v>
       </c>
@@ -2779,14 +2797,13 @@
       <c r="F15" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="G15" s="17" t="s">
-        <v>62</v>
-      </c>
       <c r="H15" s="17"/>
       <c r="I15" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="J15" s="17"/>
+      <c r="J15" s="17" t="s">
+        <v>62</v>
+      </c>
       <c r="K15" s="17" t="s">
         <v>92</v>
       </c>
@@ -2882,18 +2899,36 @@
       </c>
       <c r="L19" s="17"/>
     </row>
-    <row r="20" spans="1:12" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:12" ht="160" x14ac:dyDescent="0.15">
       <c r="A20" s="6"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
+      <c r="B20" s="14">
+        <v>17</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20" s="22">
+        <v>41223</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="G20" s="17">
+        <v>2</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>110</v>
+      </c>
       <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
+      <c r="K20" s="17" t="s">
+        <v>111</v>
+      </c>
       <c r="L20" s="17"/>
     </row>
     <row r="21" spans="1:12" ht="22" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
2nd draft cover letter
</commit_message>
<xml_diff>
--- a/List of position opennings.xlsx
+++ b/List of position opennings.xlsx
@@ -2342,10 +2342,10 @@
   <dimension ref="A1:IV23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="I19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomRight" activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>